<commit_message>
modification of test data
</commit_message>
<xml_diff>
--- a/data/test_dem_values.xlsx
+++ b/data/test_dem_values.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10740" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10740" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="dem_1" sheetId="3" r:id="rId1"/>
     <sheet name="dem_2" sheetId="1" r:id="rId2"/>
     <sheet name="dem_3" sheetId="4" r:id="rId3"/>
+    <sheet name="mask1" sheetId="5" r:id="rId4"/>
+    <sheet name="dem_2_mask1" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="9">
   <si>
     <t>min</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,13 +49,29 @@
     <t>range</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>cols</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rows</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>After set value (without the (0,0) set to 1.0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>After set value (with the (0,0) set to 1.0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="181" formatCode="0.00000000"/>
+    <numFmt numFmtId="176" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -72,12 +90,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -94,11 +118,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2175,8 +2202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3923,7 +3950,7 @@
   <dimension ref="A1:AD29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="A22" sqref="A22:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5659,4 +5686,1169 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>-9999</v>
+      </c>
+      <c r="D1">
+        <v>-9999</v>
+      </c>
+      <c r="E1">
+        <v>-9999</v>
+      </c>
+      <c r="F1">
+        <v>-9999</v>
+      </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+      <c r="J1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>-9999</v>
+      </c>
+      <c r="D2">
+        <v>-9999</v>
+      </c>
+      <c r="E2">
+        <v>-9999</v>
+      </c>
+      <c r="F2">
+        <v>-9999</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>-9999</v>
+      </c>
+      <c r="G7">
+        <v>-9999</v>
+      </c>
+      <c r="H7">
+        <v>-9999</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>-9999</v>
+      </c>
+      <c r="G8">
+        <v>-9999</v>
+      </c>
+      <c r="H8">
+        <v>-9999</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>-9999</v>
+      </c>
+      <c r="G9">
+        <v>-9999</v>
+      </c>
+      <c r="H9">
+        <v>-9999</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f>SUMIF(A1:J9,"&lt;&gt;-9999")</f>
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>7.94</v>
+      </c>
+      <c r="B1">
+        <v>7.62</v>
+      </c>
+      <c r="G1">
+        <v>9.43</v>
+      </c>
+      <c r="H1">
+        <v>9.9</v>
+      </c>
+      <c r="I1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J1">
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>9.75</v>
+      </c>
+      <c r="B2">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="C2">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="D2">
+        <v>8.83</v>
+      </c>
+      <c r="E2">
+        <v>8.77</v>
+      </c>
+      <c r="F2">
+        <v>8.31</v>
+      </c>
+      <c r="G2">
+        <v>9.33</v>
+      </c>
+      <c r="J2">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>9.64</v>
+      </c>
+      <c r="C3">
+        <v>9.75</v>
+      </c>
+      <c r="D3">
+        <v>7.14</v>
+      </c>
+      <c r="E3">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="H3">
+        <v>7.14</v>
+      </c>
+      <c r="I3">
+        <v>9.75</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>7.07</v>
+      </c>
+      <c r="B4">
+        <v>9.9</v>
+      </c>
+      <c r="C4">
+        <v>9.06</v>
+      </c>
+      <c r="D4">
+        <v>7.21</v>
+      </c>
+      <c r="E4">
+        <v>9.17</v>
+      </c>
+      <c r="F4">
+        <v>7.94</v>
+      </c>
+      <c r="G4">
+        <v>8.6</v>
+      </c>
+      <c r="H4">
+        <v>7.07</v>
+      </c>
+      <c r="I4">
+        <v>8.43</v>
+      </c>
+      <c r="J4">
+        <v>9.64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>7.28</v>
+      </c>
+      <c r="B5">
+        <v>8.43</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>9.85</v>
+      </c>
+      <c r="E5">
+        <v>9.59</v>
+      </c>
+      <c r="F5">
+        <v>7.68</v>
+      </c>
+      <c r="G5">
+        <v>8.43</v>
+      </c>
+      <c r="H5">
+        <v>8.19</v>
+      </c>
+      <c r="I5">
+        <v>9.15</v>
+      </c>
+      <c r="J5">
+        <v>8.5399999999999991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>7.75</v>
+      </c>
+      <c r="C6">
+        <v>9.59</v>
+      </c>
+      <c r="D6">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="E6">
+        <v>9.64</v>
+      </c>
+      <c r="I6">
+        <v>9.85</v>
+      </c>
+      <c r="J6">
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>7.07</v>
+      </c>
+      <c r="C7">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="D7">
+        <v>9.85</v>
+      </c>
+      <c r="E7">
+        <v>7.94</v>
+      </c>
+      <c r="I7">
+        <v>98.49</v>
+      </c>
+      <c r="J7">
+        <v>7.14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>7.81</v>
+      </c>
+      <c r="C8">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="D8">
+        <v>8.83</v>
+      </c>
+      <c r="E8">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="I8">
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="J8">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f>SUMIF(A1:J8,"&lt;&gt;-9999")</f>
+        <v>614.25999999999988</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f>COUNTIF(A1:J8,"&gt;-9999")</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f>AVERAGEIF(A1:J8,"&lt;&gt;-9999")</f>
+        <v>10.237666666666664</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
+        <f>MIN(A1:J8)</f>
+        <v>7.07</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <f>MAX(A1:J8)</f>
+        <v>98.49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1">
+        <f>AVERAGE(A1:J8)</f>
+        <v>10.237666666666664</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1">
+        <f>_xlfn.STDEV.P(A1:J8)</f>
+        <v>11.529529531694786</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1">
+        <f>B15-B14</f>
+        <v>91.419999999999987</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>7.94</v>
+      </c>
+      <c r="B21">
+        <v>7.62</v>
+      </c>
+      <c r="G21">
+        <v>9.43</v>
+      </c>
+      <c r="H21">
+        <v>9.9</v>
+      </c>
+      <c r="I21">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J21">
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>9.75</v>
+      </c>
+      <c r="B22">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="C22">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="D22">
+        <v>8.83</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.877</v>
+      </c>
+      <c r="F22">
+        <v>8.31</v>
+      </c>
+      <c r="G22">
+        <v>9.33</v>
+      </c>
+      <c r="J22">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <v>9.64</v>
+      </c>
+      <c r="C23">
+        <v>9.75</v>
+      </c>
+      <c r="D23">
+        <v>7.14</v>
+      </c>
+      <c r="E23">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="H23">
+        <v>7.14</v>
+      </c>
+      <c r="I23">
+        <v>9.75</v>
+      </c>
+      <c r="J23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>7.07</v>
+      </c>
+      <c r="B24">
+        <v>9.9</v>
+      </c>
+      <c r="C24">
+        <v>9.06</v>
+      </c>
+      <c r="D24">
+        <v>7.21</v>
+      </c>
+      <c r="E24">
+        <v>9.17</v>
+      </c>
+      <c r="F24">
+        <v>7.94</v>
+      </c>
+      <c r="G24">
+        <v>8.6</v>
+      </c>
+      <c r="H24">
+        <v>7.07</v>
+      </c>
+      <c r="I24">
+        <v>8.43</v>
+      </c>
+      <c r="J24">
+        <v>9.64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>7.28</v>
+      </c>
+      <c r="B25">
+        <v>8.43</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>9.85</v>
+      </c>
+      <c r="E25">
+        <v>9.59</v>
+      </c>
+      <c r="F25">
+        <v>7.68</v>
+      </c>
+      <c r="G25">
+        <v>8.43</v>
+      </c>
+      <c r="H25">
+        <v>8.19</v>
+      </c>
+      <c r="I25">
+        <v>9.15</v>
+      </c>
+      <c r="J25">
+        <v>8.5399999999999991</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>7.75</v>
+      </c>
+      <c r="C26">
+        <v>9.59</v>
+      </c>
+      <c r="D26">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="E26">
+        <v>9.64</v>
+      </c>
+      <c r="I26">
+        <v>9.85</v>
+      </c>
+      <c r="J26">
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>7.07</v>
+      </c>
+      <c r="C27">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="D27">
+        <v>9.85</v>
+      </c>
+      <c r="E27">
+        <v>7.94</v>
+      </c>
+      <c r="I27">
+        <v>98.49</v>
+      </c>
+      <c r="J27">
+        <v>7.14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>7.81</v>
+      </c>
+      <c r="C28">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="D28">
+        <v>8.83</v>
+      </c>
+      <c r="E28">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="I28">
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="J28">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <f>SUMIF(A21:J28,"&lt;&gt;-9999")</f>
+        <v>606.36699999999985</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <f>COUNTIF(A21:J28,"&gt;-9999")</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <f>AVERAGEIF(A21:J28,"&lt;&gt;-9999")</f>
+        <v>10.106116666666663</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1">
+        <f>MIN(A21:J28)</f>
+        <v>0.877</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1">
+        <f>MAX(A21:J28)</f>
+        <v>98.49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="1">
+        <f>AVERAGE(A21:J28)</f>
+        <v>10.106116666666663</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="1">
+        <f>_xlfn.STDEV.P(A21:J28)</f>
+        <v>11.590393136978669</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="1">
+        <f>B35-B34</f>
+        <v>97.613</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>7.94</v>
+      </c>
+      <c r="B45">
+        <v>7.62</v>
+      </c>
+      <c r="G45">
+        <v>9.43</v>
+      </c>
+      <c r="H45">
+        <v>9.9</v>
+      </c>
+      <c r="I45">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J45">
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>9.75</v>
+      </c>
+      <c r="B46">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="C46">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="D46">
+        <v>8.83</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0.877</v>
+      </c>
+      <c r="F46">
+        <v>8.31</v>
+      </c>
+      <c r="G46">
+        <v>9.33</v>
+      </c>
+      <c r="J46">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>9</v>
+      </c>
+      <c r="B47">
+        <v>9.64</v>
+      </c>
+      <c r="C47">
+        <v>9.75</v>
+      </c>
+      <c r="D47">
+        <v>7.14</v>
+      </c>
+      <c r="E47">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="H47">
+        <v>7.14</v>
+      </c>
+      <c r="I47">
+        <v>9.75</v>
+      </c>
+      <c r="J47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>7.07</v>
+      </c>
+      <c r="B48">
+        <v>9.9</v>
+      </c>
+      <c r="C48">
+        <v>9.06</v>
+      </c>
+      <c r="D48">
+        <v>7.21</v>
+      </c>
+      <c r="E48">
+        <v>9.17</v>
+      </c>
+      <c r="F48">
+        <v>7.94</v>
+      </c>
+      <c r="G48">
+        <v>8.6</v>
+      </c>
+      <c r="H48">
+        <v>7.07</v>
+      </c>
+      <c r="I48">
+        <v>8.43</v>
+      </c>
+      <c r="J48">
+        <v>9.64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>7.28</v>
+      </c>
+      <c r="B49">
+        <v>8.43</v>
+      </c>
+      <c r="C49">
+        <v>8</v>
+      </c>
+      <c r="D49">
+        <v>9.85</v>
+      </c>
+      <c r="E49">
+        <v>9.59</v>
+      </c>
+      <c r="F49">
+        <v>7.68</v>
+      </c>
+      <c r="G49">
+        <v>8.43</v>
+      </c>
+      <c r="H49">
+        <v>8.19</v>
+      </c>
+      <c r="I49">
+        <v>9.15</v>
+      </c>
+      <c r="J49">
+        <v>8.5399999999999991</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B50">
+        <v>7.75</v>
+      </c>
+      <c r="C50">
+        <v>9.59</v>
+      </c>
+      <c r="D50">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="E50">
+        <v>9.64</v>
+      </c>
+      <c r="I50">
+        <v>9.85</v>
+      </c>
+      <c r="J50">
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B51">
+        <v>7.07</v>
+      </c>
+      <c r="C51">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="D51">
+        <v>9.85</v>
+      </c>
+      <c r="E51">
+        <v>7.94</v>
+      </c>
+      <c r="I51">
+        <v>98.49</v>
+      </c>
+      <c r="J51">
+        <v>7.14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B52">
+        <v>7.81</v>
+      </c>
+      <c r="C52">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="D52">
+        <v>8.83</v>
+      </c>
+      <c r="E52">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="I52">
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="J52">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <f>SUMIF(A44:J52,"&lt;&gt;-9999")</f>
+        <v>607.36699999999985</v>
+      </c>
+      <c r="D55" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <f>COUNTIF(A44:J52,"&gt;-9999")</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <f>AVERAGEIF(A44:J52,"&lt;&gt;-9999")</f>
+        <v>9.9568360655737678</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="1">
+        <f>MIN(A44:J52)</f>
+        <v>0.877</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" s="1">
+        <f>MAX(A44:J52)</f>
+        <v>98.49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="1">
+        <f>AVERAGE(A44:J52)</f>
+        <v>9.9568360655737678</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="1">
+        <f>_xlfn.STDEV.P(A44:J52)</f>
+        <v>11.55301023746175</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="1">
+        <f>B59-B58</f>
+        <v>97.613</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add test of mongodb IO
</commit_message>
<xml_diff>
--- a/data/test_dem_values.xlsx
+++ b/data/test_dem_values.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10740" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10740" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="dem_1" sheetId="3" r:id="rId1"/>
@@ -6005,8 +6005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6859,7 +6859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>